<commit_message>
Updated dfMods.py to create additional columns. Fixed errors in which columns were labeled nominal instead of ordinal as they should be.
</commit_message>
<xml_diff>
--- a/Column Notes.xlsx
+++ b/Column Notes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -576,6 +576,15 @@
   <si>
     <t xml:space="preserve">Condition of sale</t>
   </si>
+  <si>
+    <t xml:space="preserve">SalePrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sale Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dollars</t>
+  </si>
 </sst>
 </file>
 
@@ -584,7 +593,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -622,6 +631,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -666,7 +681,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -676,6 +691,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -696,10 +715,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C80" activeCellId="0" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -821,7 +840,7 @@
         <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>4</v>
@@ -835,7 +854,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>4</v>
@@ -1560,7 +1579,7 @@
         <v>132</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>6</v>
@@ -1574,7 +1593,7 @@
         <v>134</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>6</v>
@@ -1588,7 +1607,7 @@
         <v>136</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>3</v>
@@ -1686,7 +1705,7 @@
         <v>150</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>5</v>
@@ -1700,7 +1719,7 @@
         <v>152</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>5</v>
@@ -1779,6 +1798,20 @@
       </c>
       <c r="D79" s="0" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed ImputationTrain and dfMod.py. Fixed some bugs in Column Notes.xlsx.
</commit_message>
<xml_diff>
--- a/Column Notes.xlsx
+++ b/Column Notes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="170">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Unit Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropped</t>
   </si>
   <si>
     <t xml:space="preserve">MSSubClass</t>
@@ -535,6 +538,9 @@
     <t xml:space="preserve">Pool Quality (includes NA)</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fence</t>
   </si>
   <si>
@@ -590,8 +596,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -681,7 +688,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -691,6 +698,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -715,10 +726,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C80" activeCellId="0" sqref="C80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F76" activeCellId="0" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -747,16 +758,19 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>16</v>
@@ -764,13 +778,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>8</v>
@@ -778,27 +792,27 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2</v>
@@ -806,13 +820,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
@@ -820,13 +834,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>4</v>
@@ -834,13 +848,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>4</v>
@@ -848,13 +862,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>4</v>
@@ -862,13 +876,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>5</v>
@@ -876,13 +890,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>3</v>
@@ -890,13 +904,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>25</v>
@@ -904,13 +918,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>9</v>
@@ -918,13 +932,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>9</v>
@@ -932,13 +946,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>5</v>
@@ -946,13 +960,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>8</v>
@@ -960,13 +974,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>10</v>
@@ -974,13 +988,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>10</v>
@@ -988,35 +1002,35 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>6</v>
@@ -1024,13 +1038,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>8</v>
@@ -1038,13 +1052,13 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>17</v>
@@ -1052,13 +1066,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>17</v>
@@ -1066,13 +1080,13 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>5</v>
@@ -1080,27 +1094,27 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>5</v>
@@ -1108,13 +1122,13 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>5</v>
@@ -1122,13 +1136,13 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>6</v>
@@ -1136,30 +1150,30 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>6</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>6</v>
@@ -1167,13 +1181,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>5</v>
@@ -1181,13 +1195,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>7</v>
@@ -1195,27 +1209,27 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>7</v>
@@ -1223,56 +1237,56 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>6</v>
@@ -1280,13 +1294,13 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>5</v>
@@ -1294,13 +1308,13 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>2</v>
@@ -1308,13 +1322,13 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>5</v>
@@ -1322,136 +1336,136 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>5</v>
@@ -1459,24 +1473,24 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>8</v>
@@ -1484,24 +1498,24 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>6</v>
@@ -1509,13 +1523,13 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>7</v>
@@ -1523,24 +1537,24 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>4</v>
@@ -1548,38 +1562,38 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>6</v>
@@ -1587,13 +1601,13 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>6</v>
@@ -1601,13 +1615,13 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>3</v>
@@ -1615,111 +1629,114 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="F72" s="3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>5</v>
@@ -1727,60 +1744,63 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="F74" s="0" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>10</v>
@@ -1788,30 +1808,30 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
-        <v>165</v>
+      <c r="A80" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Regressions.py. ConvergenceWarning is present on Lasso and ElasticNet regressions. Column Notes updated to include continuous variables, as well as columns made in dfMods.py.
</commit_message>
<xml_diff>
--- a/Column Notes.xlsx
+++ b/Column Notes.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Original Columns" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Additional Columns" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="181">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -61,103 +62,106 @@
     <t xml:space="preserve">Amount of street connected to property</t>
   </si>
   <si>
+    <t xml:space="preserve">Continuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of road access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of alley access to property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LotShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shape of property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordinal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LandContour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flatness of property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of utilities available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LotConfig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lot configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LandSlope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steepness of slope of property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neighborhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which neighborhood the property is in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximity to various conditions (Railroads)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same as Above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BldgType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of Building (Family Size)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HouseStyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Style of Building (# of Stories)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OverallQual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-10 rating of quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OverallCond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-10 rating of condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YearBuilt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construction date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Discrete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of road access</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of alley access to property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LotShape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shape of property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ordinal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LandContour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flatness of property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of utilities available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LotConfig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lot configuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LandSlope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steepness of slope of property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neighborhood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which neighborhood the property is in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proximity to various conditions (Railroads)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Same as Above</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BldgType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of Building (Family Size)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HouseStyle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Style of Building (# of Stories)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OverallQual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-10 rating of quality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OverallCond</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-10 rating of condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YearBuilt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Construction date</t>
   </si>
   <si>
     <t xml:space="preserve">YearRemodAdd</t>
@@ -532,15 +536,15 @@
     <t xml:space="preserve">Pool area</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoolQC</t>
   </si>
   <si>
     <t xml:space="preserve">Pool Quality (includes NA)</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fence</t>
   </si>
   <si>
@@ -590,6 +594,36 @@
   </si>
   <si>
     <t xml:space="preserve">Dollars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GarageScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GarageQual * GarageArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotalFullBath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BsmtFullBath + FullBath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotalHalfBath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BsmtHalfBath + HalfBath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotalSF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrLivArea + TotalBsmtSF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogSalePrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">np.log(SalePrice)</t>
   </si>
 </sst>
 </file>
@@ -600,7 +634,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -630,6 +664,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -688,7 +728,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -701,11 +741,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,8 +772,8 @@
   </sheetPr>
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F76" activeCellId="0" sqref="F76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E81" activeCellId="0" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1008,26 +1052,26 @@
         <v>45</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>8</v>
@@ -1038,10 +1082,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>8</v>
@@ -1052,10 +1096,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>8</v>
@@ -1066,10 +1110,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
@@ -1080,10 +1124,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>8</v>
@@ -1092,26 +1136,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>21</v>
@@ -1122,10 +1166,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
@@ -1136,10 +1180,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>8</v>
@@ -1150,10 +1194,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>21</v>
@@ -1162,15 +1206,15 @@
         <v>6</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>21</v>
@@ -1181,10 +1225,10 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>21</v>
@@ -1195,10 +1239,10 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>21</v>
@@ -1209,21 +1253,21 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>35</v>
@@ -1237,53 +1281,53 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>8</v>
@@ -1294,10 +1338,10 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>21</v>
@@ -1308,10 +1352,10 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>8</v>
@@ -1322,10 +1366,10 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>8</v>
@@ -1336,133 +1380,133 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>21</v>
@@ -1473,21 +1517,21 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>8</v>
@@ -1498,21 +1542,21 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>21</v>
@@ -1523,10 +1567,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>8</v>
@@ -1537,21 +1581,21 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>21</v>
@@ -1562,35 +1606,35 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C62" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>21</v>
@@ -1601,10 +1645,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>21</v>
@@ -1615,10 +1659,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>21</v>
@@ -1629,94 +1673,97 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="C67" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="C68" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C69" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C70" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="C71" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>21</v>
@@ -1724,16 +1771,16 @@
       <c r="D72" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>152</v>
+      <c r="F72" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>21</v>
@@ -1744,10 +1791,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>8</v>
@@ -1756,48 +1803,51 @@
         <v>6</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>13</v>
+        <v>159</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>8</v>
@@ -1808,10 +1858,10 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>8</v>
@@ -1821,17 +1871,17 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4" t="s">
-        <v>167</v>
+      <c r="A80" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="C80" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1843,4 +1893,107 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>